<commit_message>
Modification for dynamic excel report
</commit_message>
<xml_diff>
--- a/Site_Class_Report.xlsx
+++ b/Site_Class_Report.xlsx
@@ -78,7 +78,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -89,6 +89,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF59D"/>
+        <bgColor rgb="00FFF59D"/>
       </patternFill>
     </fill>
   </fills>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -272,6 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,6 +675,9 @@
           <t xml:space="preserve">Weighted Average Shear Wave Velocity VS = </t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>393.5334879869455</v>
+      </c>
       <c r="N3" s="10">
         <f>AL17</f>
         <v/>
@@ -689,7 +699,11 @@
           <t>Site Class =</t>
         </is>
       </c>
-      <c r="D4" s="1" t="n"/>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
       <c r="G4" s="17">
@@ -844,422 +858,212 @@
       <c r="AN10" s="23" t="n"/>
     </row>
     <row r="11" ht="18" customHeight="1">
-      <c r="B11" s="14" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Layer 1</t>
         </is>
       </c>
-      <c r="C11" s="20" t="n"/>
-      <c r="D11" s="21" t="n"/>
-      <c r="E11" s="5" t="n">
+      <c r="E11" t="n">
         <v>1.375</v>
       </c>
-      <c r="F11" s="20" t="n"/>
-      <c r="G11" s="20" t="n"/>
-      <c r="H11" s="21" t="n"/>
-      <c r="I11" s="5" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Saturated Sands</t>
         </is>
       </c>
-      <c r="J11" s="20" t="n"/>
-      <c r="K11" s="20" t="n"/>
-      <c r="L11" s="20" t="n"/>
-      <c r="M11" s="21" t="n"/>
-      <c r="N11" s="5" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="O11" s="20" t="n"/>
-      <c r="P11" s="21" t="n"/>
-      <c r="Q11" s="5" t="n">
+      <c r="Q11" t="n">
         <v>100</v>
       </c>
-      <c r="R11" s="20" t="n"/>
-      <c r="S11" s="21" t="n"/>
-      <c r="T11" s="5" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>80[(N1)60i]^0.4</t>
         </is>
       </c>
-      <c r="U11" s="20" t="n"/>
-      <c r="V11" s="20" t="n"/>
-      <c r="W11" s="20" t="n"/>
-      <c r="X11" s="21" t="n"/>
-      <c r="Y11" s="5" t="n">
+      <c r="Y11" t="n">
         <v>504.7658755841547</v>
       </c>
-      <c r="Z11" s="20" t="n"/>
-      <c r="AA11" s="21" t="n"/>
-      <c r="AB11" s="5" t="n">
+      <c r="AB11" t="n">
         <v>0.002724035174542538</v>
       </c>
-      <c r="AC11" s="20" t="n"/>
-      <c r="AD11" s="20" t="n"/>
-      <c r="AE11" s="21" t="n"/>
-      <c r="AG11" s="5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="AH11" s="20" t="n"/>
-      <c r="AI11" s="21" t="n"/>
-      <c r="AJ11" s="5" t="inlineStr">
-        <is>
-          <t>VS ≥ 1500</t>
-        </is>
-      </c>
-      <c r="AK11" s="20" t="n"/>
-      <c r="AL11" s="20" t="n"/>
-      <c r="AM11" s="20" t="n"/>
-      <c r="AN11" s="21" t="n"/>
     </row>
     <row r="12" ht="18" customHeight="1">
-      <c r="B12" s="14" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Layer 2</t>
         </is>
       </c>
-      <c r="C12" s="20" t="n"/>
-      <c r="D12" s="21" t="n"/>
-      <c r="E12" s="5" t="n">
+      <c r="E12" t="n">
         <v>3.2</v>
       </c>
-      <c r="F12" s="20" t="n"/>
-      <c r="G12" s="20" t="n"/>
-      <c r="H12" s="21" t="n"/>
-      <c r="I12" s="5" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Saturated Sands</t>
         </is>
       </c>
-      <c r="J12" s="20" t="n"/>
-      <c r="K12" s="20" t="n"/>
-      <c r="L12" s="20" t="n"/>
-      <c r="M12" s="21" t="n"/>
-      <c r="N12" s="5" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="O12" s="20" t="n"/>
-      <c r="P12" s="21" t="n"/>
-      <c r="Q12" s="5" t="n">
+      <c r="Q12" t="n">
         <v>15</v>
       </c>
-      <c r="R12" s="20" t="n"/>
-      <c r="S12" s="21" t="n"/>
-      <c r="T12" s="5" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>80[(N1)60i]^0.3</t>
         </is>
       </c>
-      <c r="U12" s="20" t="n"/>
-      <c r="V12" s="20" t="n"/>
-      <c r="W12" s="20" t="n"/>
-      <c r="X12" s="21" t="n"/>
-      <c r="Y12" s="5" t="n">
+      <c r="Y12" t="n">
         <v>180.2674704674124</v>
       </c>
-      <c r="Z12" s="20" t="n"/>
-      <c r="AA12" s="21" t="n"/>
-      <c r="AB12" s="5" t="n">
+      <c r="AB12" t="n">
         <v>0.017751400137267</v>
       </c>
-      <c r="AC12" s="20" t="n"/>
-      <c r="AD12" s="20" t="n"/>
-      <c r="AE12" s="21" t="n"/>
-      <c r="AG12" s="5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="AH12" s="20" t="n"/>
-      <c r="AI12" s="21" t="n"/>
-      <c r="AJ12" s="5" t="inlineStr">
-        <is>
-          <t>760 ≤ VS &lt; 1500</t>
-        </is>
-      </c>
-      <c r="AK12" s="20" t="n"/>
-      <c r="AL12" s="20" t="n"/>
-      <c r="AM12" s="20" t="n"/>
-      <c r="AN12" s="21" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1">
-      <c r="B13" s="14" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Layer 3</t>
         </is>
       </c>
-      <c r="C13" s="20" t="n"/>
-      <c r="D13" s="21" t="n"/>
-      <c r="E13" s="5" t="n">
+      <c r="E13" t="n">
         <v>2.5</v>
       </c>
-      <c r="F13" s="20" t="n"/>
-      <c r="G13" s="20" t="n"/>
-      <c r="H13" s="21" t="n"/>
-      <c r="I13" s="5" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Dry Sands</t>
         </is>
       </c>
-      <c r="J13" s="20" t="n"/>
-      <c r="K13" s="20" t="n"/>
-      <c r="L13" s="20" t="n"/>
-      <c r="M13" s="21" t="n"/>
-      <c r="N13" s="5" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="O13" s="20" t="n"/>
-      <c r="P13" s="21" t="n"/>
-      <c r="Q13" s="5" t="n">
+      <c r="Q13" t="n">
         <v>67</v>
       </c>
-      <c r="R13" s="20" t="n"/>
-      <c r="S13" s="21" t="n"/>
-      <c r="T13" s="5" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>80[(N1)60i]^0.5</t>
         </is>
       </c>
-      <c r="U13" s="20" t="n"/>
-      <c r="V13" s="20" t="n"/>
-      <c r="W13" s="20" t="n"/>
-      <c r="X13" s="21" t="n"/>
-      <c r="Y13" s="5" t="n">
+      <c r="Y13" t="n">
         <v>654.8282217497961</v>
       </c>
-      <c r="Z13" s="20" t="n"/>
-      <c r="AA13" s="21" t="n"/>
-      <c r="AB13" s="5" t="n">
+      <c r="AB13" t="n">
         <v>0.003817795136134538</v>
       </c>
-      <c r="AC13" s="20" t="n"/>
-      <c r="AD13" s="20" t="n"/>
-      <c r="AE13" s="21" t="n"/>
-      <c r="AG13" s="6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="AH13" s="20" t="n"/>
-      <c r="AI13" s="21" t="n"/>
-      <c r="AJ13" s="6" t="inlineStr">
-        <is>
-          <t>360 ≤ VS &lt; 760</t>
-        </is>
-      </c>
-      <c r="AK13" s="20" t="n"/>
-      <c r="AL13" s="20" t="n"/>
-      <c r="AM13" s="20" t="n"/>
-      <c r="AN13" s="21" t="n"/>
+      <c r="AG13" s="25" t="n"/>
+      <c r="AH13" s="25" t="n"/>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="B14" s="14" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Layer 4</t>
         </is>
       </c>
-      <c r="C14" s="20" t="n"/>
-      <c r="D14" s="21" t="n"/>
-      <c r="E14" s="5" t="n">
+      <c r="E14" t="n">
         <v>4</v>
       </c>
-      <c r="F14" s="20" t="n"/>
-      <c r="G14" s="20" t="n"/>
-      <c r="H14" s="21" t="n"/>
-      <c r="I14" s="5" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Dry Sands</t>
         </is>
       </c>
-      <c r="J14" s="20" t="n"/>
-      <c r="K14" s="20" t="n"/>
-      <c r="L14" s="20" t="n"/>
-      <c r="M14" s="21" t="n"/>
-      <c r="N14" s="5" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="O14" s="20" t="n"/>
-      <c r="P14" s="21" t="n"/>
-      <c r="Q14" s="5" t="n">
+      <c r="Q14" t="n">
         <v>53</v>
       </c>
-      <c r="R14" s="20" t="n"/>
-      <c r="S14" s="21" t="n"/>
-      <c r="T14" s="5" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>80[(N1)60i]^0.3</t>
         </is>
       </c>
-      <c r="U14" s="20" t="n"/>
-      <c r="V14" s="20" t="n"/>
-      <c r="W14" s="20" t="n"/>
-      <c r="X14" s="21" t="n"/>
-      <c r="Y14" s="5" t="n">
+      <c r="Y14" t="n">
         <v>263.2526477095353</v>
       </c>
-      <c r="Z14" s="20" t="n"/>
-      <c r="AA14" s="21" t="n"/>
-      <c r="AB14" s="5" t="n">
+      <c r="AB14" t="n">
         <v>0.01519452903817885</v>
       </c>
-      <c r="AC14" s="20" t="n"/>
-      <c r="AD14" s="20" t="n"/>
-      <c r="AE14" s="21" t="n"/>
-      <c r="AG14" s="5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AH14" s="20" t="n"/>
-      <c r="AI14" s="21" t="n"/>
-      <c r="AJ14" s="5" t="inlineStr">
-        <is>
-          <t>180 ≤ VS &lt; 360</t>
-        </is>
-      </c>
-      <c r="AK14" s="20" t="n"/>
-      <c r="AL14" s="20" t="n"/>
-      <c r="AM14" s="20" t="n"/>
-      <c r="AN14" s="21" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="B15" s="14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Layer 5</t>
         </is>
       </c>
-      <c r="C15" s="20" t="n"/>
-      <c r="D15" s="21" t="n"/>
-      <c r="E15" s="5" t="n">
+      <c r="E15" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="20" t="n"/>
-      <c r="G15" s="20" t="n"/>
-      <c r="H15" s="21" t="n"/>
-      <c r="I15" s="5" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Clays</t>
         </is>
       </c>
-      <c r="J15" s="20" t="n"/>
-      <c r="K15" s="20" t="n"/>
-      <c r="L15" s="20" t="n"/>
-      <c r="M15" s="21" t="n"/>
-      <c r="N15" s="5" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="O15" s="20" t="n"/>
-      <c r="P15" s="21" t="n"/>
-      <c r="Q15" s="5" t="n">
+      <c r="Q15" t="n">
         <v>25</v>
       </c>
-      <c r="R15" s="20" t="n"/>
-      <c r="S15" s="21" t="n"/>
-      <c r="T15" s="5" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>80[(N1)60i]^0.3</t>
         </is>
       </c>
-      <c r="U15" s="20" t="n"/>
-      <c r="V15" s="20" t="n"/>
-      <c r="W15" s="20" t="n"/>
-      <c r="X15" s="21" t="n"/>
-      <c r="Y15" s="5" t="n">
+      <c r="Y15" t="n">
         <v>210.1222243523014</v>
       </c>
-      <c r="Z15" s="20" t="n"/>
-      <c r="AA15" s="21" t="n"/>
-      <c r="AB15" s="5" t="n">
+      <c r="AB15" t="n">
         <v>0.02855480908073818</v>
       </c>
-      <c r="AC15" s="20" t="n"/>
-      <c r="AD15" s="20" t="n"/>
-      <c r="AE15" s="21" t="n"/>
-      <c r="AG15" s="5" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AH15" s="20" t="n"/>
-      <c r="AI15" s="21" t="n"/>
-      <c r="AJ15" s="5" t="inlineStr">
-        <is>
-          <t>VS ≤ 180</t>
-        </is>
-      </c>
-      <c r="AK15" s="20" t="n"/>
-      <c r="AL15" s="20" t="n"/>
-      <c r="AM15" s="20" t="n"/>
-      <c r="AN15" s="21" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="B16" s="14" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Layer 6</t>
         </is>
       </c>
-      <c r="C16" s="20" t="n"/>
-      <c r="D16" s="21" t="n"/>
-      <c r="E16" s="5" t="n">
+      <c r="E16" t="n">
         <v>10.925</v>
       </c>
-      <c r="F16" s="20" t="n"/>
-      <c r="G16" s="20" t="n"/>
-      <c r="H16" s="21" t="n"/>
-      <c r="I16" s="5" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Others</t>
         </is>
       </c>
-      <c r="J16" s="20" t="n"/>
-      <c r="K16" s="20" t="n"/>
-      <c r="L16" s="20" t="n"/>
-      <c r="M16" s="21" t="n"/>
-      <c r="N16" s="5" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="O16" s="20" t="n"/>
-      <c r="P16" s="21" t="n"/>
-      <c r="Q16" s="5" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="R16" s="20" t="n"/>
-      <c r="S16" s="21" t="n"/>
-      <c r="T16" s="5" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="U16" s="20" t="n"/>
-      <c r="V16" s="20" t="n"/>
-      <c r="W16" s="20" t="n"/>
-      <c r="X16" s="21" t="n"/>
-      <c r="Y16" s="5" t="n">
+      <c r="Y16" t="n">
         <v>3515.5</v>
       </c>
-      <c r="Z16" s="20" t="n"/>
-      <c r="AA16" s="21" t="n"/>
-      <c r="AB16" s="5" t="n">
+      <c r="AB16" t="n">
         <v>0.003107666050348457</v>
       </c>
-      <c r="AC16" s="20" t="n"/>
-      <c r="AD16" s="20" t="n"/>
-      <c r="AE16" s="21" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="B17" s="5" t="inlineStr">
@@ -1270,7 +1074,7 @@
       <c r="C17" s="20" t="n"/>
       <c r="D17" s="21" t="n"/>
       <c r="E17" s="5">
-        <f>SUM(E11:H16)</f>
+        <f>SUM(E11:E16)</f>
         <v/>
       </c>
       <c r="F17" s="20" t="n"/>
@@ -1284,7 +1088,7 @@
       <c r="Z17" s="20" t="n"/>
       <c r="AA17" s="21" t="n"/>
       <c r="AB17" s="5">
-        <f>SUM(AB11:AE16)</f>
+        <f>SUM(AB11:AB16)</f>
         <v/>
       </c>
       <c r="AC17" s="20" t="n"/>
@@ -1296,7 +1100,7 @@
         </is>
       </c>
       <c r="AL17" s="8" t="n">
-        <v>393.5334879869455</v>
+        <v>393.5335</v>
       </c>
       <c r="AN17" s="3" t="inlineStr">
         <is>
@@ -1310,10 +1114,8 @@
           <t>\</t>
         </is>
       </c>
-      <c r="AH18" s="7" t="inlineStr">
-        <is>
-          <t>Site Class =</t>
-        </is>
+      <c r="AH18" s="7" t="n">
+        <v>393.5334879869455</v>
       </c>
       <c r="AM18" s="11" t="inlineStr">
         <is>
@@ -1321,6 +1123,14 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20"/>
     <row r="21" ht="18" customHeight="1">
       <c r="AM21" s="1" t="n"/>
     </row>

</xml_diff>